<commit_message>
Correct Sakawi Takai Ciim
</commit_message>
<xml_diff>
--- a/src/data/SakawiTakaiCiim - Json.xlsx
+++ b/src/data/SakawiTakaiCiim - Json.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT PROJECTS\SakawiCham\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT PROJECTS\sakawi-cham-web\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -118,12 +118,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -153,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -165,6 +171,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +455,7 @@
   <dimension ref="A2:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,11 +814,11 @@
       <c r="G10" s="1">
         <v>2</v>
       </c>
-      <c r="H10" s="1">
-        <v>7</v>
-      </c>
-      <c r="I10" s="1">
-        <v>2</v>
+      <c r="H10" s="5">
+        <v>3</v>
+      </c>
+      <c r="I10" s="5">
+        <v>5</v>
       </c>
       <c r="J10" s="1">
         <v>6</v>

</xml_diff>